<commit_message>
Sujet Poulie réglable JP PUPIER
</commit_message>
<xml_diff>
--- a/Concevoir/03_LiaisonsEncastrementDemontables/Application_02_PoulieReglable/Barême-Poulie-Réglable.xlsx
+++ b/Concevoir/03_LiaisonsEncastrementDemontables/Application_02_PoulieReglable/Barême-Poulie-Réglable.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="B-POUREG" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'B-POUREG'!$A$1:$D$53</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
   <si>
     <t>Présentation</t>
   </si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>Vue droite</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -646,10 +652,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -831,7 +837,7 @@
       </c>
       <c r="D16" s="26"/>
     </row>
-    <row r="17" spans="1:4" ht="13.8" thickBot="1">
+    <row r="17" spans="1:7" ht="13.8" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
@@ -842,8 +848,8 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="14.4" thickTop="1" thickBot="1"/>
-    <row r="19" spans="1:4" ht="13.8" thickTop="1">
+    <row r="18" spans="1:7" ht="14.4" thickTop="1" thickBot="1"/>
+    <row r="19" spans="1:7" ht="13.8" thickTop="1">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -855,7 +861,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:7">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>4</v>
@@ -865,7 +871,7 @@
       </c>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:7">
       <c r="A21" s="4"/>
       <c r="B21" s="9" t="s">
         <v>1</v>
@@ -875,7 +881,7 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:7">
       <c r="A22" s="14" t="s">
         <v>5</v>
       </c>
@@ -887,7 +893,7 @@
       </c>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7">
       <c r="A23" s="4"/>
       <c r="B23" s="9" t="s">
         <v>4</v>
@@ -897,7 +903,7 @@
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:7">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>1</v>
@@ -907,7 +913,7 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:7">
       <c r="A25" s="14" t="s">
         <v>7</v>
       </c>
@@ -919,7 +925,7 @@
       </c>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:7">
       <c r="A26" s="18"/>
       <c r="B26" s="19" t="s">
         <v>4</v>
@@ -929,7 +935,7 @@
       </c>
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:7">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -941,7 +947,7 @@
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:7">
       <c r="A28" s="4"/>
       <c r="B28" s="22" t="s">
         <v>4</v>
@@ -951,7 +957,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:7">
       <c r="A29" s="18"/>
       <c r="B29" s="23" t="s">
         <v>1</v>
@@ -961,7 +967,7 @@
       </c>
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:7">
       <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
@@ -973,7 +979,7 @@
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:7">
       <c r="A31" s="18"/>
       <c r="B31" s="19" t="s">
         <v>4</v>
@@ -983,7 +989,7 @@
       </c>
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
@@ -994,6 +1000,9 @@
         <v>3</v>
       </c>
       <c r="D32" s="5"/>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4"/>

</xml_diff>